<commit_message>
Change ThermoFisherOrbitrap to Xcaliber
</commit_message>
<xml_diff>
--- a/data_files/ammonia_da/output/20191211003_nh3_run2.xlsx
+++ b/data_files/ammonia_da/output/20191211003_nh3_run2.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="74">
   <si>
     <t>Aliquot</t>
   </si>
@@ -104,96 +104,63 @@
     <t>NH3</t>
   </si>
   <si>
-    <t>0.002300000051036477</t>
-  </si>
-  <si>
     <t/>
   </si>
   <si>
-    <t>1</t>
-  </si>
-  <si>
     <t>4/15/2020 11:16:29 AM</t>
   </si>
   <si>
     <t>197533</t>
   </si>
   <si>
-    <t>0.019099999219179153</t>
-  </si>
-  <si>
     <t>4/15/2020 11:16:47 AM</t>
   </si>
   <si>
     <t>197534</t>
   </si>
   <si>
-    <t>0.016300000250339508</t>
-  </si>
-  <si>
     <t>4/15/2020 11:17:41 AM</t>
   </si>
   <si>
     <t>197535</t>
   </si>
   <si>
-    <t>0.002400000113993883</t>
-  </si>
-  <si>
     <t>4/15/2020 11:17:59 AM</t>
   </si>
   <si>
     <t>197536</t>
   </si>
   <si>
-    <t>0.020500000566244125</t>
-  </si>
-  <si>
     <t>4/15/2020 11:20:41 AM</t>
   </si>
   <si>
     <t>197537</t>
   </si>
   <si>
-    <t>0.019600000232458115</t>
-  </si>
-  <si>
     <t>4/15/2020 11:20:59 AM</t>
   </si>
   <si>
     <t>197538</t>
   </si>
   <si>
-    <t>0.01730000041425228</t>
-  </si>
-  <si>
     <t>4/15/2020 11:21:53 AM</t>
   </si>
   <si>
     <t>197539</t>
   </si>
   <si>
-    <t>0.021199999377131462</t>
-  </si>
-  <si>
     <t>4/15/2020 11:22:11 AM</t>
   </si>
   <si>
     <t>197540</t>
   </si>
   <si>
-    <t>0.018200000748038292</t>
-  </si>
-  <si>
     <t>4/15/2020 11:24:53 AM</t>
   </si>
   <si>
     <t>197541</t>
   </si>
   <si>
-    <t>-0.003700000001117587</t>
-  </si>
-  <si>
     <t>4/15/2020 11:25:11 AM</t>
   </si>
   <si>
@@ -203,78 +170,51 @@
     <t>197541_Dup</t>
   </si>
   <si>
-    <t>0.017999999225139618</t>
-  </si>
-  <si>
     <t>4/15/2020 11:26:05 AM</t>
   </si>
   <si>
     <t>197541_Spike</t>
   </si>
   <si>
-    <t>0.9258000254631042</t>
-  </si>
-  <si>
     <t>4/15/2020 11:29:23 AM</t>
   </si>
   <si>
     <t>BLNK</t>
   </si>
   <si>
-    <t>0.025499999523162842</t>
-  </si>
-  <si>
     <t>GFS</t>
   </si>
   <si>
-    <t>1.0311000347137451</t>
-  </si>
-  <si>
     <t>4/15/2020 11:30:17 AM</t>
   </si>
   <si>
     <t>GFS2</t>
   </si>
   <si>
-    <t>0.4821999967098236</t>
-  </si>
-  <si>
     <t>4/15/2020 11:30:35 AM</t>
   </si>
   <si>
     <t>197542</t>
   </si>
   <si>
-    <t>0.018699999898672104</t>
-  </si>
-  <si>
     <t>4/15/2020 11:33:17 AM</t>
   </si>
   <si>
     <t>197543</t>
   </si>
   <si>
-    <t>0.01940000057220459</t>
-  </si>
-  <si>
     <t>4/15/2020 11:33:35 AM</t>
   </si>
   <si>
     <t>197544</t>
   </si>
   <si>
-    <t>0.01679999940097332</t>
-  </si>
-  <si>
     <t>4/15/2020 11:34:29 AM</t>
   </si>
   <si>
     <t>197545</t>
   </si>
   <si>
-    <t>-0.017999999225139618</t>
-  </si>
-  <si>
     <t>4/15/2020 11:34:47 AM</t>
   </si>
   <si>
@@ -287,22 +227,10 @@
     <t>197545_Spike</t>
   </si>
   <si>
-    <t>0.9944000244140625</t>
-  </si>
-  <si>
     <t>4/15/2020 11:38:41 AM</t>
   </si>
   <si>
-    <t>0.026000000536441803</t>
-  </si>
-  <si>
-    <t>1.0226999521255493</t>
-  </si>
-  <si>
     <t>4/15/2020 11:39:35 AM</t>
-  </si>
-  <si>
-    <t>0.49889999628067017</t>
   </si>
   <si>
     <t>4/15/2020 11:41:41 AM</t>
@@ -450,2061 +378,2061 @@
       <c r="B2" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="0" t="s">
-        <v>30</v>
+      <c r="C2" s="0">
+        <v>0.002300000051036477</v>
       </c>
       <c r="D2" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="E2" s="0">
+        <v>1</v>
+      </c>
+      <c r="F2" s="0" t="s">
         <v>31</v>
       </c>
-      <c r="E2" s="0" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="0" t="s">
-        <v>33</v>
-      </c>
       <c r="G2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB2" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="B3" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="0" t="s">
-        <v>35</v>
+      <c r="C3" s="0">
+        <v>0.019099999219179153</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E3" s="0">
+        <v>1</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB3" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C4" s="0" t="s">
-        <v>38</v>
+      <c r="C4" s="0">
+        <v>0.016300000250339508</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E4" s="0">
+        <v>1</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB4" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="0" t="s">
-        <v>41</v>
+      <c r="C5" s="0">
+        <v>0.002400000113993883</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E5" s="0">
+        <v>1</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB5" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>43</v>
+        <v>38</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C6" s="0" t="s">
-        <v>44</v>
+      <c r="C6" s="0">
+        <v>0.020500000566244125</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E6" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E6" s="0">
+        <v>1</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB6" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>46</v>
+        <v>40</v>
       </c>
       <c r="B7" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="0" t="s">
-        <v>47</v>
+      <c r="C7" s="0">
+        <v>0.019600000232458115</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E7" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E7" s="0">
+        <v>1</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB7" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="B8" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="0" t="s">
-        <v>50</v>
+      <c r="C8" s="0">
+        <v>0.01730000041425228</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E8" s="0">
+        <v>1</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB8" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="B9" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C9" s="0" t="s">
-        <v>53</v>
+      <c r="C9" s="0">
+        <v>0.021199999377131462</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E9" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E9" s="0">
+        <v>1</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB9" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B10" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C10" s="0" t="s">
-        <v>56</v>
+      <c r="C10" s="0">
+        <v>0.018200000748038292</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E10" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E10" s="0">
+        <v>1</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB10" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="B11" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="0" t="s">
-        <v>59</v>
+      <c r="C11" s="0">
+        <v>-0.003700000001117587</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E11" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E11" s="0">
+        <v>1</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB11" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="B12" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="0" t="s">
-        <v>63</v>
+      <c r="C12" s="0">
+        <v>0.017999999225139618</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E12" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E12" s="0">
+        <v>1</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>64</v>
+        <v>52</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB12" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
       <c r="B13" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="0" t="s">
-        <v>66</v>
+      <c r="C13" s="0">
+        <v>0.9258000254631042</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E13" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E13" s="0">
+        <v>1</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB13" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B14" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C14" s="0" t="s">
-        <v>69</v>
+      <c r="C14" s="0">
+        <v>0.025499999523162842</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E14" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E14" s="0">
+        <v>1</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>67</v>
+        <v>54</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB14" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B15" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C15" s="0" t="s">
-        <v>71</v>
+      <c r="C15" s="0">
+        <v>1.0311000347137451</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E15" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E15" s="0">
+        <v>1</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>72</v>
+        <v>57</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB15" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B16" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="0" t="s">
-        <v>74</v>
+      <c r="C16" s="0">
+        <v>0.4821999967098236</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E16" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E16" s="0">
+        <v>1</v>
       </c>
       <c r="F16" s="0" t="s">
-        <v>75</v>
+        <v>59</v>
       </c>
       <c r="G16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB16" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>76</v>
+        <v>60</v>
       </c>
       <c r="B17" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C17" s="0" t="s">
-        <v>77</v>
+      <c r="C17" s="0">
+        <v>0.018699999898672104</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E17" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E17" s="0">
+        <v>1</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>78</v>
+        <v>61</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB17" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>79</v>
+        <v>62</v>
       </c>
       <c r="B18" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C18" s="0" t="s">
-        <v>80</v>
+      <c r="C18" s="0">
+        <v>0.01940000057220459</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E18" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E18" s="0">
+        <v>1</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>81</v>
+        <v>63</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB18" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="B19" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C19" s="0" t="s">
-        <v>83</v>
+      <c r="C19" s="0">
+        <v>0.01679999940097332</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E19" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E19" s="0">
+        <v>1</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>84</v>
+        <v>65</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB19" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>85</v>
+        <v>66</v>
       </c>
       <c r="B20" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C20" s="0" t="s">
-        <v>86</v>
+      <c r="C20" s="0">
+        <v>-0.017999999225139618</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E20" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E20" s="0">
+        <v>1</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB20" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="B21" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C21" s="0" t="s">
-        <v>50</v>
+      <c r="C21" s="0">
+        <v>0.01730000041425228</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E21" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E21" s="0">
+        <v>1</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB21" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="B22" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C22" s="0" t="s">
-        <v>91</v>
+      <c r="C22" s="0">
+        <v>0.9944000244140625</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E22" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E22" s="0">
+        <v>1</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB22" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>68</v>
+        <v>55</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C23" s="0" t="s">
-        <v>93</v>
+      <c r="C23" s="0">
+        <v>0.026000000536441803</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E23" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E23" s="0">
+        <v>1</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>92</v>
+        <v>71</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB23" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>70</v>
+        <v>56</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C24" s="0" t="s">
-        <v>94</v>
+      <c r="C24" s="0">
+        <v>1.0226999521255493</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E24" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E24" s="0">
+        <v>1</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>95</v>
+        <v>72</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB24" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>73</v>
+        <v>58</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="0" t="s">
-        <v>96</v>
+      <c r="C25" s="0">
+        <v>0.49889999628067017</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>31</v>
-      </c>
-      <c r="E25" s="0" t="s">
-        <v>32</v>
+        <v>30</v>
+      </c>
+      <c r="E25" s="0">
+        <v>1</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>97</v>
+        <v>73</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="J25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="K25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="L25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="M25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="P25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Q25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="R25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="S25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="T25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="U25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="V25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="W25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="X25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Y25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="Z25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AA25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="AB25" s="0" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>